<commit_message>
Add mas censistas a lista larga
</commit_message>
<xml_diff>
--- a/src/listas_de_censistas/lista_de_censistas_larga.xlsx
+++ b/src/listas_de_censistas/lista_de_censistas_larga.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Nombre</t>
   </si>
@@ -27,12 +27,6 @@
     <t>Foto</t>
   </si>
   <si>
-    <t>Julia</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
     <t>Bart</t>
   </si>
   <si>
@@ -48,10 +42,28 @@
     <t>Bob</t>
   </si>
   <si>
-    <t>Ricardo</t>
-  </si>
-  <si>
     <t>Krusty</t>
+  </si>
+  <si>
+    <t>Hibbert</t>
+  </si>
+  <si>
+    <t>Gorgory</t>
+  </si>
+  <si>
+    <t>Maggie</t>
+  </si>
+  <si>
+    <t>Moe</t>
+  </si>
+  <si>
+    <t>Ned</t>
+  </si>
+  <si>
+    <t>Skinner</t>
+  </si>
+  <si>
+    <t>Barney</t>
   </si>
 </sst>
 </file>
@@ -98,14 +110,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -129,28 +142,28 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:colOff>180109</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>213013</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1085663</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>1112086</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1070262</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPr id="8" name="Imagen 7"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -160,8 +173,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2028825" y="285750"/>
-          <a:ext cx="866588" cy="552450"/>
+          <a:off x="1998518" y="386195"/>
+          <a:ext cx="931977" cy="857249"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -173,19 +186,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>277091</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>1076620</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>962892</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPr id="9" name="Imagen 8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -194,7 +207,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -204,8 +217,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2124075" y="1019175"/>
-          <a:ext cx="628650" cy="628650"/>
+          <a:off x="2008909" y="1766455"/>
+          <a:ext cx="886120" cy="685801"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -217,19 +230,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>189634</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>193965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1011464</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>970684</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1098839</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3"/>
+        <xdr:cNvPr id="10" name="Imagen 9"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -238,7 +251,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -248,8 +261,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2095500" y="1857375"/>
-          <a:ext cx="725714" cy="457200"/>
+          <a:off x="2008043" y="2999510"/>
+          <a:ext cx="781050" cy="904874"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -261,19 +274,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>148936</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>119496</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>1168111</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1119621</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4"/>
+        <xdr:cNvPr id="32" name="Imagen 31"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -282,7 +295,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -292,8 +305,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2133600" y="2609850"/>
-          <a:ext cx="619125" cy="523875"/>
+          <a:off x="1967345" y="4241223"/>
+          <a:ext cx="1019175" cy="1000125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -305,19 +318,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>283815</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>201757</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>143731</xdr:rowOff>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1154257</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -335,9 +348,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2093565" y="3295650"/>
-          <a:ext cx="659160" cy="658081"/>
+        <a:xfrm>
+          <a:off x="2018434" y="5639666"/>
+          <a:ext cx="952500" cy="952500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -349,19 +362,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
+      <xdr:colOff>187904</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>264967</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>1311854</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>989436</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -379,9 +392,9 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2124075" y="4105274"/>
-          <a:ext cx="666750" cy="438151"/>
+        <a:xfrm>
+          <a:off x="2006313" y="7019058"/>
+          <a:ext cx="1123950" cy="724469"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -393,19 +406,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:colOff>125556</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>261505</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1217727</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:colOff>1209025</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1128280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagen 7"/>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -424,8 +437,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2095500" y="4924426"/>
-          <a:ext cx="931977" cy="400050"/>
+          <a:off x="1943965" y="8331778"/>
+          <a:ext cx="1083469" cy="866775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -437,19 +450,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:colOff>112570</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>319520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1051509</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:colOff>1255570</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1167245</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Imagen 8"/>
+        <xdr:cNvPr id="5" name="Imagen 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -468,8 +481,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2105025" y="5629276"/>
-          <a:ext cx="756234" cy="514350"/>
+          <a:off x="1930979" y="9705975"/>
+          <a:ext cx="1143000" cy="847725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -481,19 +494,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
+      <xdr:colOff>145474</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>158462</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:colOff>1269424</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1177637</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Imagen 9"/>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -512,8 +525,184 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2162175" y="6362701"/>
-          <a:ext cx="542925" cy="476250"/>
+          <a:off x="1963883" y="10861098"/>
+          <a:ext cx="1123950" cy="1019175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>370610</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>178379</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1084520</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1177638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2189019" y="12197197"/>
+          <a:ext cx="713910" cy="999259"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>239858</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>122092</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1011383</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1213718</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2058267" y="13457092"/>
+          <a:ext cx="771525" cy="1091626"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>280555</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>244186</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1033030</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1122348</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagen 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2098964" y="14895368"/>
+          <a:ext cx="752475" cy="878162"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>120361</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1000124</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1244311</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagen 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2113683" y="16087725"/>
+          <a:ext cx="704850" cy="1123950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -788,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,7 +989,7 @@
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -808,190 +997,259 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="1"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="1"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="1"/>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="1"/>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="1"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="1"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="1"/>
+      <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="1"/>
+      <c r="B28" s="3"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="1"/>
+      <c r="B29" s="3"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="1"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="1"/>
+      <c r="B31" s="3"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="1"/>
+      <c r="B32" s="3"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="1"/>
+      <c r="B33" s="3"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="1"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="3"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="1"/>
+      <c r="B35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="1"/>
+      <c r="B36" s="3"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="1"/>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2"/>
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2"/>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2"/>
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>